<commit_message>
07-11-2024 - Actualización EDAs
</commit_message>
<xml_diff>
--- a/datasets/1. Originales/dictionarys/Diccionario de Datos.xlsx
+++ b/datasets/1. Originales/dictionarys/Diccionario de Datos.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="TLC Trip Record Data" sheetId="4" r:id="rId1"/>
     <sheet name="TLC Aggregated DataMetric" sheetId="6" r:id="rId2"/>
     <sheet name="Air Quality Index" sheetId="7" r:id="rId3"/>
-    <sheet name="Otros datasets" sheetId="1" r:id="rId4"/>
+    <sheet name="Vehículos Alternativos y Electr" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="211">
   <si>
     <t>Alternative Fuel Vehicles US</t>
   </si>
@@ -38,24 +38,6 @@
     <t>City</t>
   </si>
   <si>
-    <t>ElectricCarData_Clean</t>
-  </si>
-  <si>
-    <t>LocationID</t>
-  </si>
-  <si>
-    <t>Borough</t>
-  </si>
-  <si>
-    <t>Zone</t>
-  </si>
-  <si>
-    <t>service_zone</t>
-  </si>
-  <si>
-    <t>taxi+_zone_lookup</t>
-  </si>
-  <si>
     <t>VendorID</t>
   </si>
   <si>
@@ -675,13 +657,16 @@
   </si>
   <si>
     <t xml:space="preserve">Precio del coche en euros                                             </t>
+  </si>
+  <si>
+    <t>ElectricCarData_Clean / ElectricCarData_Norm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -710,6 +695,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -719,7 +711,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -745,17 +737,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -771,12 +789,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1059,7 +1077,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -1076,526 +1094,526 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+        <v>77</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F8" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" t="s">
         <v>62</v>
       </c>
-      <c r="E9" t="s">
-        <v>62</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9" t="s">
+        <v>65</v>
+      </c>
+      <c r="J9" t="s">
+        <v>66</v>
+      </c>
+      <c r="K9" t="s">
+        <v>67</v>
+      </c>
+      <c r="L9" t="s">
         <v>68</v>
-      </c>
-      <c r="G9" t="s">
-        <v>69</v>
-      </c>
-      <c r="H9" t="s">
-        <v>70</v>
-      </c>
-      <c r="I9" t="s">
-        <v>71</v>
-      </c>
-      <c r="J9" t="s">
-        <v>72</v>
-      </c>
-      <c r="K9" t="s">
-        <v>73</v>
-      </c>
-      <c r="L9" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F10" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E11" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F11" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E12" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F12" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G12" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E13" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F13" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
         <v>56</v>
       </c>
-      <c r="B14" t="s">
-        <v>62</v>
-      </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E14" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F14" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>80</v>
+        <v>5</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="7"/>
+        <v>25</v>
+      </c>
+      <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" s="7"/>
+        <v>28</v>
+      </c>
+      <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E18" s="3"/>
-      <c r="F18" s="7"/>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E19" s="3"/>
-      <c r="F19" s="7"/>
+      <c r="F19" s="11"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E20" s="3"/>
-      <c r="F20" s="7"/>
+      <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E21" s="3"/>
-      <c r="F21" s="7"/>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E22" s="3"/>
-      <c r="F22" s="7"/>
+      <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E23" s="3"/>
-      <c r="F23" s="7"/>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E24" s="3"/>
-      <c r="F24" s="7"/>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E25" s="3"/>
-      <c r="F25" s="7"/>
+      <c r="F25" s="11"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E26" s="3"/>
-      <c r="F26" s="7"/>
+      <c r="F26" s="11"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E27" s="3"/>
-      <c r="F27" s="7"/>
+      <c r="F27" s="11"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E28" s="3"/>
-      <c r="F28" s="7"/>
+      <c r="F28" s="11"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E29" s="3"/>
-      <c r="F29" s="7"/>
+      <c r="F29" s="11"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E30" s="3"/>
-      <c r="F30" s="7"/>
+      <c r="F30" s="11"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E31" s="3"/>
-      <c r="F31" s="7"/>
+      <c r="F31" s="11"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E32" s="5"/>
-      <c r="F32" s="8"/>
+      <c r="F32" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1623,114 +1641,114 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B9" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B10" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B11" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B12" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B13" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B14" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1754,26 +1772,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1781,104 +1799,104 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B8" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B9" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B10" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B11" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B12" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>138</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>139</v>
+        <v>132</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>140</v>
-      </c>
-      <c r="B14" s="10"/>
+        <v>134</v>
+      </c>
+      <c r="B14" s="14"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>141</v>
-      </c>
-      <c r="B15" s="10"/>
+        <v>135</v>
+      </c>
+      <c r="B15" s="14"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>142</v>
-      </c>
-      <c r="B16" s="10"/>
+        <v>136</v>
+      </c>
+      <c r="B16" s="14"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>143</v>
-      </c>
-      <c r="B17" s="10"/>
+        <v>137</v>
+      </c>
+      <c r="B17" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1890,10 +1908,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D17"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1906,335 +1924,318 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
+      <c r="B1" s="17"/>
+      <c r="C1" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" t="s">
+        <v>186</v>
+      </c>
+      <c r="D7" t="s">
+        <v>200</v>
+      </c>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B8" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="C8" t="s">
+        <v>187</v>
+      </c>
+      <c r="D8" t="s">
+        <v>201</v>
+      </c>
+      <c r="E8" s="16"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B9" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C9" t="s">
         <v>188</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D9" t="s">
         <v>202</v>
       </c>
-      <c r="E4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="13"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B10" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C10" t="s">
         <v>189</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D10" t="s">
         <v>203</v>
       </c>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="13"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B11" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C11" t="s">
         <v>190</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D11" t="s">
         <v>204</v>
       </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="13"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B12" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C12" t="s">
         <v>191</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D12" t="s">
         <v>205</v>
       </c>
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="13"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B13" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C13" t="s">
         <v>192</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D13" t="s">
         <v>206</v>
       </c>
-      <c r="G8" s="13"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B14" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C14" t="s">
         <v>193</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D14" t="s">
         <v>207</v>
       </c>
-      <c r="G9" s="13"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="C15" t="s">
+        <v>194</v>
+      </c>
+      <c r="D15" t="s">
+        <v>208</v>
+      </c>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="C10" t="s">
-        <v>194</v>
-      </c>
-      <c r="D10" t="s">
-        <v>208</v>
-      </c>
-      <c r="G10" s="13"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="B16" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="C16" t="s">
+        <v>195</v>
+      </c>
+      <c r="D16" t="s">
+        <v>209</v>
+      </c>
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="C11" t="s">
-        <v>195</v>
-      </c>
-      <c r="D11" t="s">
-        <v>209</v>
-      </c>
-      <c r="G11" s="13"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="B17" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="C12" t="s">
-        <v>196</v>
-      </c>
-      <c r="D12" t="s">
-        <v>210</v>
-      </c>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="B18" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="C13" t="s">
-        <v>197</v>
-      </c>
-      <c r="D13" t="s">
-        <v>211</v>
-      </c>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="B19" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="G19" s="8"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="C14" t="s">
-        <v>198</v>
-      </c>
-      <c r="D14" t="s">
-        <v>212</v>
-      </c>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="B20" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="G20" s="8"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="B15" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="C15" t="s">
-        <v>199</v>
-      </c>
-      <c r="D15" t="s">
-        <v>213</v>
-      </c>
-      <c r="G15" s="13"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="11" t="s">
+      <c r="B21" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="C16" t="s">
-        <v>200</v>
-      </c>
-      <c r="D16" t="s">
-        <v>214</v>
-      </c>
-      <c r="G16" s="13"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B22" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="C17" t="s">
-        <v>201</v>
-      </c>
-      <c r="D17" t="s">
-        <v>215</v>
-      </c>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B23" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="G18" s="13"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B24" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="G19" s="13"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="B20" t="s">
-        <v>161</v>
-      </c>
-      <c r="G20" s="13"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="G21" s="13"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="G22" s="13"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="G23" s="13"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="G24" s="13"/>
+      <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="G25" s="12"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>